<commit_message>
Edit to match Crosswalk v14
Cells highlighted in yellow are cells where it has to be fixed in Andrew's code to generate the same file.
</commit_message>
<xml_diff>
--- a/resources/model_parameters/ModelParameters.xlsx
+++ b/resources/model_parameters/ModelParameters.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="22416"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savethong/PAVIR/Visual/TeamDataTables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350441C1-48A9-9742-99A3-80D720A8AE74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="5300" windowWidth="14680" windowHeight="15540" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="24880" windowHeight="15820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCParams" sheetId="1" r:id="rId1"/>
@@ -23,20 +29,20 @@
     <definedName name="sta3n">[1]Control!$D$2</definedName>
     <definedName name="stations">OFFSET([1]Hidden!$B$1,0,0,COUNTA([1]Hidden!$B:$B),1)</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="215">
   <si>
     <t>An estimate of the median total weekly number of psychotherapy appointments available with this team. The estimate is calculated using the volume of psychotherapy visits completed with the team over one year. (appt/wk)</t>
   </si>
@@ -161,15 +167,9 @@
     <t>An estimate of the team's appointment slots allocated to each diagnosis for clinics where the provider does not have a DEA X waiver. Evidence-based pharmacotherapy for OUD is not possible in these slots. (pct)</t>
   </si>
   <si>
-    <t>Slots Allocation (without X waiver)</t>
-  </si>
-  <si>
     <t>An estimate of the team's appointment slots allocated to each diagnosis for clinics where the provider has a DEA X waiver. Evidence-based pharmacotherapy for OUD is possible in these slots. (pct)</t>
   </si>
   <si>
-    <t>Slots Allocation (with X waiver)</t>
-  </si>
-  <si>
     <t>These estimates were calculated directly from the visit timelines of the patient cohort.  For each patient in the cohort, their first and last medication management visits were found and subtracted to get an engagement time in weeks.  Note that the first visit could be years ago, and the last visit could be the day before the query was run. Also, note that gaps in treatment are bridged, regardless of how long the gap is. See the DataNotes tab for details on the patient cohort and the encounter type bins.</t>
   </si>
   <si>
@@ -215,27 +215,15 @@
     <t>An estimate of the proportion of the team's patients with opioid use disorder (OUD), calculated from the cohort of patients who completed visits charted with a primary diagnosis of OUD within the patient's first three months.</t>
   </si>
   <si>
-    <t>%OUD within 3 months</t>
-  </si>
-  <si>
     <t>An estimate of the proportion of the team's patients with alcohol use disorder (AUD), calculated from the cohort of patients who completed visits charted with a primary diagnosis of AUD within the patient's first three months.</t>
   </si>
   <si>
-    <t>%AUD within 3 months</t>
-  </si>
-  <si>
     <t>An estimate of the proportion of the team's patients with depression (DEP), calculated from the cohort of patients who completed visits charted with a primary diagnosis of DEP within the patient's first three months.</t>
   </si>
   <si>
-    <t>%Dep within 3 months</t>
-  </si>
-  <si>
     <t>An estimate of the proportion of the team's patients with post traumatic stress disorder (PTSD), calculated from the cohort of patients who completed visits charted with a primary diagnosis of PTSD within the patient's first three months.</t>
   </si>
   <si>
-    <t>%PTSD within 3 months</t>
-  </si>
-  <si>
     <t>An estimate of the proportion of the team's patients with opioid use disorder (OUD), calculated from the cohort of patients who completed visits charted with a primary diagnosis of OUD within their entire psychotherapy engagement.</t>
   </si>
   <si>
@@ -251,9 +239,6 @@
     <t>An estimate of the proportion of the team's patients with depression (DEP), calculated from the cohort of patients who completed visits charted with a primary diagnosis of DEP within their entire psychotherapy engagement.</t>
   </si>
   <si>
-    <t>%Dep</t>
-  </si>
-  <si>
     <t>These diagnostic proportions are estimated from the patient cohort (see the DataNotes tab for details) by simply counting how many patients have a visit with the given primary diagnosis and then dividing by the cohort size. Note that the proportions can and should sum to more than one, because many patients have multiple diagnoses and get care for each in different visits which are they coded with different primary diagnoses.</t>
   </si>
   <si>
@@ -491,18 +476,12 @@
     <t>The median return-to-clinic visit interval by encounter type bin with this team, calculated from the number of visits per patient over their entire engagement time. (wks)</t>
   </si>
   <si>
-    <t>Return Visit Interval</t>
-  </si>
-  <si>
     <t>These estimates were calculated from the visit timelines of the patient cohort. For each "new patient" (see new patient start rate below for details), their first visit was found, and all visits within three months after that visit were broken out into the encounter bins. These referral percentages are the proportions of the different services (encounter type bins) received within that window, per "new patient." The referral percentage for intakes is set to 1, based on the idea that the decision about what services the patient should get is an "intake/evaluation" or review visit in the model, regardless of how that visit was actually coded. Note that this is different from the appointment supply number shown above, which does use the CPT codes on visits. See the DataNotes tab for details on the patient cohort and the encounter type bins.</t>
   </si>
   <si>
     <t>The proportion of patients who receive visits for each service with this team. Note that the percentages sum to more than one, because patients may engage in multiple services concurrently. (pct)</t>
   </si>
   <si>
-    <t>Referral Percentage</t>
-  </si>
-  <si>
     <t>These estimates were calculated directly from the visit timelines of the patient cohort.  For each patient, their first and last visits of each type were found and subtracted to get an engagement time in weeks. The engagement times shown are for the median patient.  Note that the first visit could be years ago, and the last visit could be the day before the query was run. Also, note that gaps in treatment are bridged, regardless of how long the gap is. See the DataNotes tab for details on the patient cohort and the encounter type bins.</t>
   </si>
   <si>
@@ -515,9 +494,6 @@
     <t>An estimate of the weekly hours available with this team for each service.   The estimate is calculated using the volume of visits for each service with this team over one year. (appt/wk)</t>
   </si>
   <si>
-    <t>Appointment Supply</t>
-  </si>
-  <si>
     <t>These estimates were calculated from the visits and appointments of the patient cohort.  Note that missed appointments do not have an associated visit record, and so do not have an encounter type. Therefore, these missed appointment percentages by encounter type bin were estimated by using patient characteristics: all the patients who had had a visit of a certain encounter type with this team have all their missed appointments counted towards that encounter type. See the DataNotes tab for details on the patient cohort and the encounter type bins.</t>
   </si>
   <si>
@@ -675,13 +651,205 @@
   </si>
   <si>
     <t>New Patient Wait Time (wks)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Slots Allocation </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (with X waiver)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Slots Allocation</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve"> %</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (without X waiver)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">New Patient Start Rate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>(mean)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Appointment Supply </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>(median)</t>
+    </r>
+  </si>
+  <si>
+    <t>Service Proportions from Team Data</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Return Visit Interval </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>(median)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PTSD within 3 months </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AUD within 3 months </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OUD within 3 months </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>%D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>EP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>EP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> within 3 months </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Initiators Who Quit Early </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Duration</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,8 +920,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,6 +943,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -846,7 +1037,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -976,6 +1167,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1003,7 +1199,7 @@
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1019,7 +1215,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Control"/>
@@ -2104,22 +2300,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.83203125" customWidth="1"/>
     <col min="3" max="3" width="126" style="2" customWidth="1"/>
@@ -2128,7 +2324,7 @@
     <col min="10" max="10" width="94.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="32">
       <c r="A1" s="7" t="s">
         <v>31</v>
       </c>
@@ -2142,7 +2338,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="16">
       <c r="A2" s="14" t="s">
         <v>28</v>
       </c>
@@ -2153,7 +2349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="32">
       <c r="A3" s="11" t="s">
         <v>26</v>
       </c>
@@ -2167,7 +2363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28">
+    <row r="4" spans="1:4" ht="32">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -2181,7 +2377,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="32">
       <c r="A5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2195,7 +2391,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28">
+    <row r="6" spans="1:4" ht="32">
       <c r="A6" s="10" t="s">
         <v>18</v>
       </c>
@@ -2206,7 +2402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="16">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -2217,7 +2413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28">
+    <row r="8" spans="1:4" ht="32">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -2231,7 +2427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28">
+    <row r="9" spans="1:4" ht="32">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -2245,7 +2441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28">
+    <row r="10" spans="1:4" ht="32">
       <c r="A10" s="11" t="s">
         <v>10</v>
       </c>
@@ -2259,7 +2455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="42">
+    <row r="11" spans="1:4" ht="48">
       <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
@@ -2273,7 +2469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="42">
+    <row r="12" spans="1:4" ht="48">
       <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
@@ -2287,7 +2483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="16">
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2313,15 +2509,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="109.5" style="16" customWidth="1"/>
@@ -2331,7 +2527,7 @@
     <col min="10" max="10" width="94.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:9" ht="32">
       <c r="A1" s="7" t="s">
         <v>31</v>
       </c>
@@ -2348,7 +2544,7 @@
         <v>0.13</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>29</v>
@@ -2371,12 +2567,12 @@
         <v>0.75</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="23"/>
     </row>
-    <row r="3" spans="1:9" ht="28">
+    <row r="3" spans="1:9" ht="32">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
@@ -2393,13 +2589,13 @@
         <v>0.19</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="28">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="32">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -2416,13 +2612,13 @@
         <v>40</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28">
+    <row r="5" spans="1:9" ht="32">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -2439,13 +2635,13 @@
         <v>40</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28">
+    <row r="6" spans="1:9" ht="32">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2462,11 +2658,11 @@
         <v>1</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="28">
+    <row r="7" spans="1:9" ht="32">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -2483,11 +2679,11 @@
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="28">
+    <row r="8" spans="1:9" ht="32">
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
@@ -2504,13 +2700,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28">
+    <row r="9" spans="1:9" ht="32">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2527,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>8</v>
@@ -2550,13 +2746,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="42">
+    <row r="11" spans="1:9" ht="48">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2573,13 +2769,13 @@
         <v>69</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="42">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="48">
       <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
@@ -2596,15 +2792,15 @@
         <v>69</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="28">
-      <c r="A13" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="32">
+      <c r="A13" s="63" t="s">
+        <v>203</v>
       </c>
       <c r="B13" s="6">
         <v>0</v>
@@ -2619,15 +2815,15 @@
         <v>0.92</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28">
-      <c r="A14" s="7" t="s">
-        <v>41</v>
+    <row r="14" spans="1:9" ht="32">
+      <c r="A14" s="63" t="s">
+        <v>204</v>
       </c>
       <c r="B14" s="6">
         <v>0</v>
@@ -2648,7 +2844,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28">
+    <row r="15" spans="1:9" ht="32">
       <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
@@ -2681,7 +2877,7 @@
       </c>
       <c r="F16" s="17"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" ht="16">
       <c r="F18" s="3" t="s">
         <v>2</v>
       </c>
@@ -2708,15 +2904,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="55.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.33203125" customWidth="1"/>
@@ -2730,116 +2926,116 @@
     <col min="10" max="10" width="94.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="16">
       <c r="A2" s="34" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="42">
+    <row r="3" spans="1:6" ht="48">
       <c r="A3" s="53" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C3" s="19">
         <v>0.1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="42">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="48">
       <c r="A4" s="53"/>
       <c r="B4" s="19" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C4" s="19">
         <v>0.18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="32">
       <c r="A5" s="53"/>
       <c r="B5" s="19" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C5" s="19">
         <v>0.06</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E5" s="48"/>
     </row>
-    <row r="6" spans="1:6" ht="42">
+    <row r="6" spans="1:6" ht="48">
       <c r="A6" s="53"/>
       <c r="B6" s="19" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C6" s="19">
         <v>0.76</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="28">
+    <row r="7" spans="1:6" ht="32">
       <c r="A7" s="54"/>
       <c r="B7" s="19" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C7" s="19">
         <v>0.35</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E7" s="48"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="55" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C8" s="29">
         <v>1</v>
       </c>
       <c r="D8" s="57" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="56"/>
       <c r="B9" s="33" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C9" s="33">
         <v>2</v>
@@ -2851,7 +3047,7 @@
     <row r="10" spans="1:6">
       <c r="A10" s="56"/>
       <c r="B10" s="33" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C10" s="33">
         <v>2</v>
@@ -2862,7 +3058,7 @@
     <row r="11" spans="1:6">
       <c r="A11" s="56"/>
       <c r="B11" s="33" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C11" s="19">
         <v>1</v>
@@ -2873,7 +3069,7 @@
     <row r="12" spans="1:6">
       <c r="A12" s="56"/>
       <c r="B12" s="33" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C12" s="19">
         <v>1</v>
@@ -2883,21 +3079,21 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="56"/>
-      <c r="B13" s="33" t="s">
-        <v>109</v>
+      <c r="B13" s="67" t="s">
+        <v>214</v>
       </c>
       <c r="C13" s="19">
         <v>2</v>
       </c>
       <c r="D13" s="57" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="54"/>
       <c r="B14" s="33" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C14" s="19">
         <v>8</v>
@@ -2907,25 +3103,25 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="55" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C15" s="29">
         <v>18</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="56"/>
       <c r="B16" s="33" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C16" s="33">
         <v>15</v>
@@ -2936,7 +3132,7 @@
     <row r="17" spans="1:5">
       <c r="A17" s="56"/>
       <c r="B17" s="33" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C17" s="30">
         <v>7</v>
@@ -2947,7 +3143,7 @@
     <row r="18" spans="1:5">
       <c r="A18" s="56"/>
       <c r="B18" s="29" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C18" s="29">
         <v>4</v>
@@ -2958,7 +3154,7 @@
     <row r="19" spans="1:5">
       <c r="A19" s="56"/>
       <c r="B19" s="33" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C19" s="33">
         <v>4</v>
@@ -2969,7 +3165,7 @@
     <row r="20" spans="1:5">
       <c r="A20" s="56"/>
       <c r="B20" s="33" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C20" s="30">
         <v>4</v>
@@ -2980,7 +3176,7 @@
     <row r="21" spans="1:5">
       <c r="A21" s="56"/>
       <c r="B21" s="29" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C21" s="29">
         <v>2</v>
@@ -2991,7 +3187,7 @@
     <row r="22" spans="1:5">
       <c r="A22" s="56"/>
       <c r="B22" s="33" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C22" s="19">
         <v>2</v>
@@ -3002,7 +3198,7 @@
     <row r="23" spans="1:5">
       <c r="A23" s="56"/>
       <c r="B23" s="33" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C23" s="19">
         <v>3</v>
@@ -3013,20 +3209,20 @@
     <row r="24" spans="1:5">
       <c r="A24" s="56"/>
       <c r="B24" s="29" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C24" s="29">
         <v>36</v>
       </c>
       <c r="D24" s="57" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E24" s="48"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="56"/>
       <c r="B25" s="33" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C25" s="19">
         <v>76</v>
@@ -3037,7 +3233,7 @@
     <row r="26" spans="1:5">
       <c r="A26" s="56"/>
       <c r="B26" s="33" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C26" s="19">
         <v>104</v>
@@ -3048,7 +3244,7 @@
     <row r="27" spans="1:5">
       <c r="A27" s="56"/>
       <c r="B27" s="29" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C27" s="29">
         <v>14</v>
@@ -3059,7 +3255,7 @@
     <row r="28" spans="1:5">
       <c r="A28" s="56"/>
       <c r="B28" s="33" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C28" s="19">
         <v>33</v>
@@ -3070,7 +3266,7 @@
     <row r="29" spans="1:5">
       <c r="A29" s="56"/>
       <c r="B29" s="33" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C29" s="19">
         <v>66</v>
@@ -3081,7 +3277,7 @@
     <row r="30" spans="1:5">
       <c r="A30" s="56"/>
       <c r="B30" s="29" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C30" s="29">
         <v>12</v>
@@ -3092,7 +3288,7 @@
     <row r="31" spans="1:5">
       <c r="A31" s="56"/>
       <c r="B31" s="33" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C31" s="19">
         <v>29</v>
@@ -3103,7 +3299,7 @@
     <row r="32" spans="1:5">
       <c r="A32" s="54"/>
       <c r="B32" s="33" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C32" s="19">
         <v>53</v>
@@ -3111,26 +3307,26 @@
       <c r="D32" s="57"/>
       <c r="E32" s="48"/>
     </row>
-    <row r="33" spans="1:5" ht="28">
+    <row r="33" spans="1:5" ht="32">
       <c r="A33" s="32" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C33" s="29">
         <v>4.25</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="42">
+    <row r="34" spans="1:5" ht="48">
       <c r="A34" s="49" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>14</v>
@@ -3145,7 +3341,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="28">
+    <row r="35" spans="1:5" ht="48">
       <c r="A35" s="50"/>
       <c r="B35" s="28" t="s">
         <v>12</v>
@@ -3160,7 +3356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28">
+    <row r="36" spans="1:5" ht="32">
       <c r="A36" s="51"/>
       <c r="B36" s="30" t="s">
         <v>10</v>
@@ -3169,27 +3365,27 @@
         <v>64</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="28">
+    <row r="37" spans="1:5" ht="32">
       <c r="A37" s="49" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C37" s="29">
         <v>388</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3210,111 +3406,111 @@
       <c r="D39" s="26"/>
       <c r="E39" s="25"/>
     </row>
-    <row r="40" spans="1:5" ht="42">
+    <row r="40" spans="1:5" ht="48">
       <c r="A40" s="49" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C40">
         <v>0.97</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E40" s="48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="42">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="48">
       <c r="A41" s="52"/>
-      <c r="B41" t="s">
-        <v>71</v>
+      <c r="B41" s="66" t="s">
+        <v>212</v>
       </c>
       <c r="C41">
         <v>0.05</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E41" s="48"/>
     </row>
-    <row r="42" spans="1:5" ht="42">
+    <row r="42" spans="1:5" ht="48">
       <c r="A42" s="52"/>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E42" s="48"/>
     </row>
-    <row r="43" spans="1:5" ht="42">
+    <row r="43" spans="1:5" ht="48">
       <c r="A43" s="52"/>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E43" s="48"/>
     </row>
-    <row r="44" spans="1:5" ht="42">
+    <row r="44" spans="1:5" ht="48">
       <c r="A44" s="52"/>
-      <c r="B44" t="s">
-        <v>65</v>
+      <c r="B44" s="66" t="s">
+        <v>209</v>
       </c>
       <c r="C44">
         <v>0.97</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E44" s="48"/>
     </row>
-    <row r="45" spans="1:5" ht="28">
+    <row r="45" spans="1:5" ht="32">
       <c r="A45" s="52"/>
-      <c r="B45" t="s">
-        <v>63</v>
+      <c r="B45" s="66" t="s">
+        <v>213</v>
       </c>
       <c r="C45">
         <v>0.05</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E45" s="48"/>
     </row>
-    <row r="46" spans="1:5" ht="28">
+    <row r="46" spans="1:5" ht="48">
       <c r="A46" s="52"/>
-      <c r="B46" t="s">
-        <v>61</v>
+      <c r="B46" s="66" t="s">
+        <v>210</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E46" s="48"/>
     </row>
-    <row r="47" spans="1:5" ht="28">
+    <row r="47" spans="1:5" ht="48">
       <c r="A47" s="52"/>
-      <c r="B47" t="s">
-        <v>59</v>
+      <c r="B47" s="66" t="s">
+        <v>211</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E47" s="48"/>
     </row>
@@ -3345,15 +3541,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet10" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33.5" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="8.83203125" style="35"/>
@@ -3364,7 +3560,7 @@
     <col min="13" max="16384" width="8.83203125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="70">
+    <row r="1" spans="1:14" ht="80">
       <c r="A1" s="19" t="s">
         <v>26</v>
       </c>
@@ -3390,15 +3586,15 @@
         <v>0.18</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="84">
-      <c r="A2" s="19" t="s">
-        <v>159</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="96">
+      <c r="A2" s="64" t="s">
+        <v>206</v>
       </c>
       <c r="B2" s="19">
         <v>3</v>
@@ -3422,13 +3618,13 @@
         <v>2</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="J2" s="44" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="98">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="112">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -3454,15 +3650,15 @@
         <v>19</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="J3" s="44" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="98">
-      <c r="A4" s="19" t="s">
-        <v>154</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="112">
+      <c r="A4" s="65" t="s">
+        <v>207</v>
       </c>
       <c r="B4" s="19">
         <v>1</v>
@@ -3486,15 +3682,15 @@
         <v>0.15</v>
       </c>
       <c r="I4" s="43" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="J4" s="44" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="56">
-      <c r="A5" s="19" t="s">
-        <v>151</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="80">
+      <c r="A5" s="64" t="s">
+        <v>208</v>
       </c>
       <c r="B5" s="19">
         <v>1</v>
@@ -3518,15 +3714,15 @@
         <v>2</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J5" s="44" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="126">
-      <c r="A6" s="19" t="s">
-        <v>83</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="144">
+      <c r="A6" s="64" t="s">
+        <v>205</v>
       </c>
       <c r="B6" s="19">
         <v>9.3800000000000008</v>
@@ -3550,15 +3746,15 @@
         <v>0</v>
       </c>
       <c r="I6" s="43" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="J6" s="42" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="33" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B7" s="33">
         <v>0</v>
@@ -3583,12 +3779,12 @@
       </c>
       <c r="I7" s="57"/>
       <c r="J7" s="58" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="33" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B8" s="33">
         <v>7.0000000000000007E-2</v>
@@ -3616,7 +3812,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="33" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B9" s="33">
         <v>0</v>
@@ -3644,7 +3840,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="33" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B10" s="33">
         <v>0.91</v>
@@ -3676,7 +3872,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="30" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B11" s="33">
         <v>0.57999999999999996</v>
@@ -3708,28 +3904,28 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="41" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="I12" s="39"/>
       <c r="J12" s="39"/>
@@ -3869,15 +4065,15 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet16" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.83203125" style="46" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
@@ -3886,41 +4082,41 @@
     <col min="5" max="5" width="78.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="16">
       <c r="A1" s="46" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E1" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1">
       <c r="A2" s="60" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C2" s="47">
         <v>6.7692300000000003</v>
       </c>
       <c r="D2" s="61" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20.25" customHeight="1">
       <c r="A3" s="60"/>
       <c r="B3" s="47" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C3" s="47">
         <v>1.0384610000000001</v>
@@ -3931,7 +4127,7 @@
     <row r="4" spans="1:5" ht="20.25" customHeight="1">
       <c r="A4" s="60"/>
       <c r="B4" s="47" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C4" s="47">
         <v>9.6153000000000002E-2</v>
@@ -3941,25 +4137,25 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="60" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C5" s="47">
         <v>5.7692E-2</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="60"/>
       <c r="B6" s="47" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C6" s="47">
         <v>0.115384</v>
@@ -3970,7 +4166,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="60"/>
       <c r="B7" s="47" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C7" s="47">
         <v>1.9230000000000001E-2</v>
@@ -3980,25 +4176,25 @@
     </row>
     <row r="8" spans="1:5" ht="32.25" customHeight="1">
       <c r="A8" s="60" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C8" s="47">
         <v>37.428570999999998</v>
       </c>
       <c r="D8" s="61" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="32.25" customHeight="1">
       <c r="A9" s="60"/>
       <c r="B9" s="47" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C9" s="47">
         <v>25.428570999999998</v>
@@ -4009,7 +4205,7 @@
     <row r="10" spans="1:5" ht="32.25" customHeight="1">
       <c r="A10" s="60"/>
       <c r="B10" s="47" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C10" s="47">
         <v>43.428570999999998</v>
@@ -4019,25 +4215,25 @@
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1">
       <c r="A11" s="60" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C11" s="47">
         <v>44.071427999999997</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="60"/>
       <c r="B12" s="47" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C12" s="47">
         <v>4.8571419999999996</v>
@@ -4048,7 +4244,7 @@
     <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="A13" s="60"/>
       <c r="B13" s="47" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C13" s="47">
         <v>0</v>
@@ -4058,25 +4254,25 @@
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1">
       <c r="A14" s="60" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C14" s="47">
         <v>45.571427999999997</v>
       </c>
       <c r="D14" s="61" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E14" s="62" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1">
       <c r="A15" s="60"/>
       <c r="B15" s="47" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C15" s="47">
         <v>68</v>
@@ -4087,7 +4283,7 @@
     <row r="16" spans="1:5" ht="18.75" customHeight="1">
       <c r="A16" s="60"/>
       <c r="B16" s="47" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C16" s="47">
         <v>48.714284999999997</v>
@@ -4098,7 +4294,7 @@
     <row r="17" spans="1:5" ht="18.75" customHeight="1">
       <c r="A17" s="60"/>
       <c r="B17" s="47" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C17" s="47">
         <v>18.714285</v>
@@ -4109,7 +4305,7 @@
     <row r="18" spans="1:5" ht="18.75" customHeight="1">
       <c r="A18" s="60"/>
       <c r="B18" s="47" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C18" s="47">
         <v>14.571427999999999</v>
@@ -4120,7 +4316,7 @@
     <row r="19" spans="1:5" ht="18.75" customHeight="1">
       <c r="A19" s="60"/>
       <c r="B19" s="47" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C19" s="47">
         <v>62</v>
@@ -4130,25 +4326,25 @@
     </row>
     <row r="20" spans="1:5" ht="28.5" customHeight="1">
       <c r="A20" s="60" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C20" s="47">
         <v>37.428570999999998</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="28.5" customHeight="1">
       <c r="A21" s="60"/>
       <c r="B21" s="47" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C21" s="47">
         <v>44.928571000000005</v>
@@ -4159,7 +4355,7 @@
     <row r="22" spans="1:5" ht="28.5" customHeight="1">
       <c r="A22" s="60"/>
       <c r="B22" s="47" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C22" s="47">
         <v>68.142857000000006</v>
@@ -4169,25 +4365,25 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="60" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B23" s="47" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C23" s="47">
         <v>22.142856999999999</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="E23" s="62" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="60"/>
       <c r="B24" s="47" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C24" s="47">
         <v>28</v>
@@ -4198,7 +4394,7 @@
     <row r="25" spans="1:5">
       <c r="A25" s="60"/>
       <c r="B25" s="47" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C25" s="47">
         <v>27</v>
@@ -4209,7 +4405,7 @@
     <row r="26" spans="1:5">
       <c r="A26" s="60"/>
       <c r="B26" s="47" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C26" s="47">
         <v>14.642856500000001</v>
@@ -4220,7 +4416,7 @@
     <row r="27" spans="1:5">
       <c r="A27" s="60"/>
       <c r="B27" s="47" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C27" s="47">
         <v>39.571427999999997</v>
@@ -4231,7 +4427,7 @@
     <row r="28" spans="1:5">
       <c r="A28" s="60"/>
       <c r="B28" s="47" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C28" s="47">
         <v>6.571428</v>
@@ -4241,25 +4437,25 @@
     </row>
     <row r="29" spans="1:5" ht="38.25" customHeight="1">
       <c r="A29" s="60" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C29" s="47">
         <v>0.45488721804499999</v>
       </c>
       <c r="D29" s="61" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="38.25" customHeight="1">
       <c r="A30" s="60"/>
       <c r="B30" s="47" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C30" s="47">
         <v>3.8004750593E-2</v>
@@ -4270,7 +4466,7 @@
     <row r="31" spans="1:5" ht="38.25" customHeight="1">
       <c r="A31" s="60"/>
       <c r="B31" s="47" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C31" s="47">
         <v>5.6338028169E-2</v>
@@ -4280,10 +4476,10 @@
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1">
       <c r="A32" s="60" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -4292,7 +4488,7 @@
     <row r="33" spans="1:3">
       <c r="A33" s="60"/>
       <c r="B33" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C33">
         <v>52</v>
@@ -4301,7 +4497,7 @@
     <row r="34" spans="1:3">
       <c r="A34" s="60"/>
       <c r="B34" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C34">
         <v>10</v>
@@ -4309,10 +4505,10 @@
     </row>
     <row r="35" spans="1:3" ht="45" customHeight="1">
       <c r="A35" s="60" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B35" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -4321,7 +4517,7 @@
     <row r="36" spans="1:3">
       <c r="A36" s="60"/>
       <c r="B36" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -4330,7 +4526,7 @@
     <row r="37" spans="1:3">
       <c r="A37" s="60"/>
       <c r="B37" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -4338,10 +4534,10 @@
     </row>
     <row r="38" spans="1:3" ht="30" customHeight="1">
       <c r="A38" s="60" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B38" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -4350,7 +4546,7 @@
     <row r="39" spans="1:3">
       <c r="A39" s="60"/>
       <c r="B39" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -4358,10 +4554,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="60" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B40" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C40">
         <v>4</v>
@@ -4370,7 +4566,7 @@
     <row r="41" spans="1:3">
       <c r="A41" s="60"/>
       <c r="B41" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -4379,7 +4575,7 @@
     <row r="42" spans="1:3">
       <c r="A42" s="60"/>
       <c r="B42" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C42">
         <v>4</v>
@@ -4387,19 +4583,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="A29:A31"/>
     <mergeCell ref="E29:E31"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="E11:E13"/>
@@ -4409,12 +4598,19 @@
     <mergeCell ref="E14:E19"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E23:E28"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Edit to match Crosswalk v14 (#236)
Cells highlighted in yellow are cells where it has to be fixed in Andrew's code to generate the same file.
</commit_message>
<xml_diff>
--- a/resources/model_parameters/ModelParameters.xlsx
+++ b/resources/model_parameters/ModelParameters.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="22416"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savethong/PAVIR/Visual/TeamDataTables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350441C1-48A9-9742-99A3-80D720A8AE74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="5300" windowWidth="14680" windowHeight="15540" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="24880" windowHeight="15820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCParams" sheetId="1" r:id="rId1"/>
@@ -23,20 +29,20 @@
     <definedName name="sta3n">[1]Control!$D$2</definedName>
     <definedName name="stations">OFFSET([1]Hidden!$B$1,0,0,COUNTA([1]Hidden!$B:$B),1)</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="215">
   <si>
     <t>An estimate of the median total weekly number of psychotherapy appointments available with this team. The estimate is calculated using the volume of psychotherapy visits completed with the team over one year. (appt/wk)</t>
   </si>
@@ -161,15 +167,9 @@
     <t>An estimate of the team's appointment slots allocated to each diagnosis for clinics where the provider does not have a DEA X waiver. Evidence-based pharmacotherapy for OUD is not possible in these slots. (pct)</t>
   </si>
   <si>
-    <t>Slots Allocation (without X waiver)</t>
-  </si>
-  <si>
     <t>An estimate of the team's appointment slots allocated to each diagnosis for clinics where the provider has a DEA X waiver. Evidence-based pharmacotherapy for OUD is possible in these slots. (pct)</t>
   </si>
   <si>
-    <t>Slots Allocation (with X waiver)</t>
-  </si>
-  <si>
     <t>These estimates were calculated directly from the visit timelines of the patient cohort.  For each patient in the cohort, their first and last medication management visits were found and subtracted to get an engagement time in weeks.  Note that the first visit could be years ago, and the last visit could be the day before the query was run. Also, note that gaps in treatment are bridged, regardless of how long the gap is. See the DataNotes tab for details on the patient cohort and the encounter type bins.</t>
   </si>
   <si>
@@ -215,27 +215,15 @@
     <t>An estimate of the proportion of the team's patients with opioid use disorder (OUD), calculated from the cohort of patients who completed visits charted with a primary diagnosis of OUD within the patient's first three months.</t>
   </si>
   <si>
-    <t>%OUD within 3 months</t>
-  </si>
-  <si>
     <t>An estimate of the proportion of the team's patients with alcohol use disorder (AUD), calculated from the cohort of patients who completed visits charted with a primary diagnosis of AUD within the patient's first three months.</t>
   </si>
   <si>
-    <t>%AUD within 3 months</t>
-  </si>
-  <si>
     <t>An estimate of the proportion of the team's patients with depression (DEP), calculated from the cohort of patients who completed visits charted with a primary diagnosis of DEP within the patient's first three months.</t>
   </si>
   <si>
-    <t>%Dep within 3 months</t>
-  </si>
-  <si>
     <t>An estimate of the proportion of the team's patients with post traumatic stress disorder (PTSD), calculated from the cohort of patients who completed visits charted with a primary diagnosis of PTSD within the patient's first three months.</t>
   </si>
   <si>
-    <t>%PTSD within 3 months</t>
-  </si>
-  <si>
     <t>An estimate of the proportion of the team's patients with opioid use disorder (OUD), calculated from the cohort of patients who completed visits charted with a primary diagnosis of OUD within their entire psychotherapy engagement.</t>
   </si>
   <si>
@@ -251,9 +239,6 @@
     <t>An estimate of the proportion of the team's patients with depression (DEP), calculated from the cohort of patients who completed visits charted with a primary diagnosis of DEP within their entire psychotherapy engagement.</t>
   </si>
   <si>
-    <t>%Dep</t>
-  </si>
-  <si>
     <t>These diagnostic proportions are estimated from the patient cohort (see the DataNotes tab for details) by simply counting how many patients have a visit with the given primary diagnosis and then dividing by the cohort size. Note that the proportions can and should sum to more than one, because many patients have multiple diagnoses and get care for each in different visits which are they coded with different primary diagnoses.</t>
   </si>
   <si>
@@ -491,18 +476,12 @@
     <t>The median return-to-clinic visit interval by encounter type bin with this team, calculated from the number of visits per patient over their entire engagement time. (wks)</t>
   </si>
   <si>
-    <t>Return Visit Interval</t>
-  </si>
-  <si>
     <t>These estimates were calculated from the visit timelines of the patient cohort. For each "new patient" (see new patient start rate below for details), their first visit was found, and all visits within three months after that visit were broken out into the encounter bins. These referral percentages are the proportions of the different services (encounter type bins) received within that window, per "new patient." The referral percentage for intakes is set to 1, based on the idea that the decision about what services the patient should get is an "intake/evaluation" or review visit in the model, regardless of how that visit was actually coded. Note that this is different from the appointment supply number shown above, which does use the CPT codes on visits. See the DataNotes tab for details on the patient cohort and the encounter type bins.</t>
   </si>
   <si>
     <t>The proportion of patients who receive visits for each service with this team. Note that the percentages sum to more than one, because patients may engage in multiple services concurrently. (pct)</t>
   </si>
   <si>
-    <t>Referral Percentage</t>
-  </si>
-  <si>
     <t>These estimates were calculated directly from the visit timelines of the patient cohort.  For each patient, their first and last visits of each type were found and subtracted to get an engagement time in weeks. The engagement times shown are for the median patient.  Note that the first visit could be years ago, and the last visit could be the day before the query was run. Also, note that gaps in treatment are bridged, regardless of how long the gap is. See the DataNotes tab for details on the patient cohort and the encounter type bins.</t>
   </si>
   <si>
@@ -515,9 +494,6 @@
     <t>An estimate of the weekly hours available with this team for each service.   The estimate is calculated using the volume of visits for each service with this team over one year. (appt/wk)</t>
   </si>
   <si>
-    <t>Appointment Supply</t>
-  </si>
-  <si>
     <t>These estimates were calculated from the visits and appointments of the patient cohort.  Note that missed appointments do not have an associated visit record, and so do not have an encounter type. Therefore, these missed appointment percentages by encounter type bin were estimated by using patient characteristics: all the patients who had had a visit of a certain encounter type with this team have all their missed appointments counted towards that encounter type. See the DataNotes tab for details on the patient cohort and the encounter type bins.</t>
   </si>
   <si>
@@ -675,13 +651,205 @@
   </si>
   <si>
     <t>New Patient Wait Time (wks)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Slots Allocation </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (with X waiver)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Slots Allocation</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve"> %</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (without X waiver)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">New Patient Start Rate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>(mean)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Appointment Supply </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>(median)</t>
+    </r>
+  </si>
+  <si>
+    <t>Service Proportions from Team Data</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Return Visit Interval </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>(median)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PTSD within 3 months </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AUD within 3 months </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OUD within 3 months </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>%D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>EP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>EP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> within 3 months </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Initiators Who Quit Early </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Duration</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,8 +920,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,6 +943,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -846,7 +1037,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -976,6 +1167,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1003,7 +1199,7 @@
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1019,7 +1215,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Control"/>
@@ -2104,22 +2300,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.83203125" customWidth="1"/>
     <col min="3" max="3" width="126" style="2" customWidth="1"/>
@@ -2128,7 +2324,7 @@
     <col min="10" max="10" width="94.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="32">
       <c r="A1" s="7" t="s">
         <v>31</v>
       </c>
@@ -2142,7 +2338,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="16">
       <c r="A2" s="14" t="s">
         <v>28</v>
       </c>
@@ -2153,7 +2349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="32">
       <c r="A3" s="11" t="s">
         <v>26</v>
       </c>
@@ -2167,7 +2363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28">
+    <row r="4" spans="1:4" ht="32">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -2181,7 +2377,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="32">
       <c r="A5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2195,7 +2391,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28">
+    <row r="6" spans="1:4" ht="32">
       <c r="A6" s="10" t="s">
         <v>18</v>
       </c>
@@ -2206,7 +2402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="16">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -2217,7 +2413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28">
+    <row r="8" spans="1:4" ht="32">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -2231,7 +2427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28">
+    <row r="9" spans="1:4" ht="32">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -2245,7 +2441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28">
+    <row r="10" spans="1:4" ht="32">
       <c r="A10" s="11" t="s">
         <v>10</v>
       </c>
@@ -2259,7 +2455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="42">
+    <row r="11" spans="1:4" ht="48">
       <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
@@ -2273,7 +2469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="42">
+    <row r="12" spans="1:4" ht="48">
       <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
@@ -2287,7 +2483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="16">
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2313,15 +2509,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="109.5" style="16" customWidth="1"/>
@@ -2331,7 +2527,7 @@
     <col min="10" max="10" width="94.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:9" ht="32">
       <c r="A1" s="7" t="s">
         <v>31</v>
       </c>
@@ -2348,7 +2544,7 @@
         <v>0.13</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>29</v>
@@ -2371,12 +2567,12 @@
         <v>0.75</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="23"/>
     </row>
-    <row r="3" spans="1:9" ht="28">
+    <row r="3" spans="1:9" ht="32">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
@@ -2393,13 +2589,13 @@
         <v>0.19</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="28">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="32">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -2416,13 +2612,13 @@
         <v>40</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28">
+    <row r="5" spans="1:9" ht="32">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -2439,13 +2635,13 @@
         <v>40</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28">
+    <row r="6" spans="1:9" ht="32">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2462,11 +2658,11 @@
         <v>1</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="28">
+    <row r="7" spans="1:9" ht="32">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -2483,11 +2679,11 @@
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="28">
+    <row r="8" spans="1:9" ht="32">
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
@@ -2504,13 +2700,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28">
+    <row r="9" spans="1:9" ht="32">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2527,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>8</v>
@@ -2550,13 +2746,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="42">
+    <row r="11" spans="1:9" ht="48">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2573,13 +2769,13 @@
         <v>69</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="42">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="48">
       <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
@@ -2596,15 +2792,15 @@
         <v>69</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="28">
-      <c r="A13" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="32">
+      <c r="A13" s="63" t="s">
+        <v>203</v>
       </c>
       <c r="B13" s="6">
         <v>0</v>
@@ -2619,15 +2815,15 @@
         <v>0.92</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28">
-      <c r="A14" s="7" t="s">
-        <v>41</v>
+    <row r="14" spans="1:9" ht="32">
+      <c r="A14" s="63" t="s">
+        <v>204</v>
       </c>
       <c r="B14" s="6">
         <v>0</v>
@@ -2648,7 +2844,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28">
+    <row r="15" spans="1:9" ht="32">
       <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
@@ -2681,7 +2877,7 @@
       </c>
       <c r="F16" s="17"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" ht="16">
       <c r="F18" s="3" t="s">
         <v>2</v>
       </c>
@@ -2708,15 +2904,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="55.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.33203125" customWidth="1"/>
@@ -2730,116 +2926,116 @@
     <col min="10" max="10" width="94.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="16">
       <c r="A2" s="34" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="42">
+    <row r="3" spans="1:6" ht="48">
       <c r="A3" s="53" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C3" s="19">
         <v>0.1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="42">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="48">
       <c r="A4" s="53"/>
       <c r="B4" s="19" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C4" s="19">
         <v>0.18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="32">
       <c r="A5" s="53"/>
       <c r="B5" s="19" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C5" s="19">
         <v>0.06</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E5" s="48"/>
     </row>
-    <row r="6" spans="1:6" ht="42">
+    <row r="6" spans="1:6" ht="48">
       <c r="A6" s="53"/>
       <c r="B6" s="19" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C6" s="19">
         <v>0.76</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="28">
+    <row r="7" spans="1:6" ht="32">
       <c r="A7" s="54"/>
       <c r="B7" s="19" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C7" s="19">
         <v>0.35</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E7" s="48"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="55" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C8" s="29">
         <v>1</v>
       </c>
       <c r="D8" s="57" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="56"/>
       <c r="B9" s="33" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C9" s="33">
         <v>2</v>
@@ -2851,7 +3047,7 @@
     <row r="10" spans="1:6">
       <c r="A10" s="56"/>
       <c r="B10" s="33" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C10" s="33">
         <v>2</v>
@@ -2862,7 +3058,7 @@
     <row r="11" spans="1:6">
       <c r="A11" s="56"/>
       <c r="B11" s="33" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C11" s="19">
         <v>1</v>
@@ -2873,7 +3069,7 @@
     <row r="12" spans="1:6">
       <c r="A12" s="56"/>
       <c r="B12" s="33" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C12" s="19">
         <v>1</v>
@@ -2883,21 +3079,21 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="56"/>
-      <c r="B13" s="33" t="s">
-        <v>109</v>
+      <c r="B13" s="67" t="s">
+        <v>214</v>
       </c>
       <c r="C13" s="19">
         <v>2</v>
       </c>
       <c r="D13" s="57" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="54"/>
       <c r="B14" s="33" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C14" s="19">
         <v>8</v>
@@ -2907,25 +3103,25 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="55" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C15" s="29">
         <v>18</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="56"/>
       <c r="B16" s="33" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C16" s="33">
         <v>15</v>
@@ -2936,7 +3132,7 @@
     <row r="17" spans="1:5">
       <c r="A17" s="56"/>
       <c r="B17" s="33" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C17" s="30">
         <v>7</v>
@@ -2947,7 +3143,7 @@
     <row r="18" spans="1:5">
       <c r="A18" s="56"/>
       <c r="B18" s="29" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C18" s="29">
         <v>4</v>
@@ -2958,7 +3154,7 @@
     <row r="19" spans="1:5">
       <c r="A19" s="56"/>
       <c r="B19" s="33" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C19" s="33">
         <v>4</v>
@@ -2969,7 +3165,7 @@
     <row r="20" spans="1:5">
       <c r="A20" s="56"/>
       <c r="B20" s="33" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C20" s="30">
         <v>4</v>
@@ -2980,7 +3176,7 @@
     <row r="21" spans="1:5">
       <c r="A21" s="56"/>
       <c r="B21" s="29" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C21" s="29">
         <v>2</v>
@@ -2991,7 +3187,7 @@
     <row r="22" spans="1:5">
       <c r="A22" s="56"/>
       <c r="B22" s="33" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C22" s="19">
         <v>2</v>
@@ -3002,7 +3198,7 @@
     <row r="23" spans="1:5">
       <c r="A23" s="56"/>
       <c r="B23" s="33" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C23" s="19">
         <v>3</v>
@@ -3013,20 +3209,20 @@
     <row r="24" spans="1:5">
       <c r="A24" s="56"/>
       <c r="B24" s="29" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C24" s="29">
         <v>36</v>
       </c>
       <c r="D24" s="57" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E24" s="48"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="56"/>
       <c r="B25" s="33" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C25" s="19">
         <v>76</v>
@@ -3037,7 +3233,7 @@
     <row r="26" spans="1:5">
       <c r="A26" s="56"/>
       <c r="B26" s="33" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C26" s="19">
         <v>104</v>
@@ -3048,7 +3244,7 @@
     <row r="27" spans="1:5">
       <c r="A27" s="56"/>
       <c r="B27" s="29" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C27" s="29">
         <v>14</v>
@@ -3059,7 +3255,7 @@
     <row r="28" spans="1:5">
       <c r="A28" s="56"/>
       <c r="B28" s="33" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C28" s="19">
         <v>33</v>
@@ -3070,7 +3266,7 @@
     <row r="29" spans="1:5">
       <c r="A29" s="56"/>
       <c r="B29" s="33" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C29" s="19">
         <v>66</v>
@@ -3081,7 +3277,7 @@
     <row r="30" spans="1:5">
       <c r="A30" s="56"/>
       <c r="B30" s="29" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C30" s="29">
         <v>12</v>
@@ -3092,7 +3288,7 @@
     <row r="31" spans="1:5">
       <c r="A31" s="56"/>
       <c r="B31" s="33" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C31" s="19">
         <v>29</v>
@@ -3103,7 +3299,7 @@
     <row r="32" spans="1:5">
       <c r="A32" s="54"/>
       <c r="B32" s="33" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C32" s="19">
         <v>53</v>
@@ -3111,26 +3307,26 @@
       <c r="D32" s="57"/>
       <c r="E32" s="48"/>
     </row>
-    <row r="33" spans="1:5" ht="28">
+    <row r="33" spans="1:5" ht="32">
       <c r="A33" s="32" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C33" s="29">
         <v>4.25</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="42">
+    <row r="34" spans="1:5" ht="48">
       <c r="A34" s="49" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>14</v>
@@ -3145,7 +3341,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="28">
+    <row r="35" spans="1:5" ht="48">
       <c r="A35" s="50"/>
       <c r="B35" s="28" t="s">
         <v>12</v>
@@ -3160,7 +3356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28">
+    <row r="36" spans="1:5" ht="32">
       <c r="A36" s="51"/>
       <c r="B36" s="30" t="s">
         <v>10</v>
@@ -3169,27 +3365,27 @@
         <v>64</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="28">
+    <row r="37" spans="1:5" ht="32">
       <c r="A37" s="49" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C37" s="29">
         <v>388</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3210,111 +3406,111 @@
       <c r="D39" s="26"/>
       <c r="E39" s="25"/>
     </row>
-    <row r="40" spans="1:5" ht="42">
+    <row r="40" spans="1:5" ht="48">
       <c r="A40" s="49" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C40">
         <v>0.97</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E40" s="48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="42">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="48">
       <c r="A41" s="52"/>
-      <c r="B41" t="s">
-        <v>71</v>
+      <c r="B41" s="66" t="s">
+        <v>212</v>
       </c>
       <c r="C41">
         <v>0.05</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E41" s="48"/>
     </row>
-    <row r="42" spans="1:5" ht="42">
+    <row r="42" spans="1:5" ht="48">
       <c r="A42" s="52"/>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E42" s="48"/>
     </row>
-    <row r="43" spans="1:5" ht="42">
+    <row r="43" spans="1:5" ht="48">
       <c r="A43" s="52"/>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E43" s="48"/>
     </row>
-    <row r="44" spans="1:5" ht="42">
+    <row r="44" spans="1:5" ht="48">
       <c r="A44" s="52"/>
-      <c r="B44" t="s">
-        <v>65</v>
+      <c r="B44" s="66" t="s">
+        <v>209</v>
       </c>
       <c r="C44">
         <v>0.97</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E44" s="48"/>
     </row>
-    <row r="45" spans="1:5" ht="28">
+    <row r="45" spans="1:5" ht="32">
       <c r="A45" s="52"/>
-      <c r="B45" t="s">
-        <v>63</v>
+      <c r="B45" s="66" t="s">
+        <v>213</v>
       </c>
       <c r="C45">
         <v>0.05</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E45" s="48"/>
     </row>
-    <row r="46" spans="1:5" ht="28">
+    <row r="46" spans="1:5" ht="48">
       <c r="A46" s="52"/>
-      <c r="B46" t="s">
-        <v>61</v>
+      <c r="B46" s="66" t="s">
+        <v>210</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E46" s="48"/>
     </row>
-    <row r="47" spans="1:5" ht="28">
+    <row r="47" spans="1:5" ht="48">
       <c r="A47" s="52"/>
-      <c r="B47" t="s">
-        <v>59</v>
+      <c r="B47" s="66" t="s">
+        <v>211</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E47" s="48"/>
     </row>
@@ -3345,15 +3541,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet10" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33.5" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="8.83203125" style="35"/>
@@ -3364,7 +3560,7 @@
     <col min="13" max="16384" width="8.83203125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="70">
+    <row r="1" spans="1:14" ht="80">
       <c r="A1" s="19" t="s">
         <v>26</v>
       </c>
@@ -3390,15 +3586,15 @@
         <v>0.18</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="84">
-      <c r="A2" s="19" t="s">
-        <v>159</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="96">
+      <c r="A2" s="64" t="s">
+        <v>206</v>
       </c>
       <c r="B2" s="19">
         <v>3</v>
@@ -3422,13 +3618,13 @@
         <v>2</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="J2" s="44" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="98">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="112">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -3454,15 +3650,15 @@
         <v>19</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="J3" s="44" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="98">
-      <c r="A4" s="19" t="s">
-        <v>154</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="112">
+      <c r="A4" s="65" t="s">
+        <v>207</v>
       </c>
       <c r="B4" s="19">
         <v>1</v>
@@ -3486,15 +3682,15 @@
         <v>0.15</v>
       </c>
       <c r="I4" s="43" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="J4" s="44" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="56">
-      <c r="A5" s="19" t="s">
-        <v>151</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="80">
+      <c r="A5" s="64" t="s">
+        <v>208</v>
       </c>
       <c r="B5" s="19">
         <v>1</v>
@@ -3518,15 +3714,15 @@
         <v>2</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J5" s="44" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="126">
-      <c r="A6" s="19" t="s">
-        <v>83</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="144">
+      <c r="A6" s="64" t="s">
+        <v>205</v>
       </c>
       <c r="B6" s="19">
         <v>9.3800000000000008</v>
@@ -3550,15 +3746,15 @@
         <v>0</v>
       </c>
       <c r="I6" s="43" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="J6" s="42" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="33" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B7" s="33">
         <v>0</v>
@@ -3583,12 +3779,12 @@
       </c>
       <c r="I7" s="57"/>
       <c r="J7" s="58" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="33" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B8" s="33">
         <v>7.0000000000000007E-2</v>
@@ -3616,7 +3812,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="33" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B9" s="33">
         <v>0</v>
@@ -3644,7 +3840,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="33" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B10" s="33">
         <v>0.91</v>
@@ -3676,7 +3872,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="30" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B11" s="33">
         <v>0.57999999999999996</v>
@@ -3708,28 +3904,28 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="41" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="I12" s="39"/>
       <c r="J12" s="39"/>
@@ -3869,15 +4065,15 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet16" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.83203125" style="46" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
@@ -3886,41 +4082,41 @@
     <col min="5" max="5" width="78.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="16">
       <c r="A1" s="46" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E1" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1">
       <c r="A2" s="60" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C2" s="47">
         <v>6.7692300000000003</v>
       </c>
       <c r="D2" s="61" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20.25" customHeight="1">
       <c r="A3" s="60"/>
       <c r="B3" s="47" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C3" s="47">
         <v>1.0384610000000001</v>
@@ -3931,7 +4127,7 @@
     <row r="4" spans="1:5" ht="20.25" customHeight="1">
       <c r="A4" s="60"/>
       <c r="B4" s="47" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C4" s="47">
         <v>9.6153000000000002E-2</v>
@@ -3941,25 +4137,25 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="60" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C5" s="47">
         <v>5.7692E-2</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="60"/>
       <c r="B6" s="47" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C6" s="47">
         <v>0.115384</v>
@@ -3970,7 +4166,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="60"/>
       <c r="B7" s="47" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C7" s="47">
         <v>1.9230000000000001E-2</v>
@@ -3980,25 +4176,25 @@
     </row>
     <row r="8" spans="1:5" ht="32.25" customHeight="1">
       <c r="A8" s="60" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C8" s="47">
         <v>37.428570999999998</v>
       </c>
       <c r="D8" s="61" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="32.25" customHeight="1">
       <c r="A9" s="60"/>
       <c r="B9" s="47" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C9" s="47">
         <v>25.428570999999998</v>
@@ -4009,7 +4205,7 @@
     <row r="10" spans="1:5" ht="32.25" customHeight="1">
       <c r="A10" s="60"/>
       <c r="B10" s="47" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C10" s="47">
         <v>43.428570999999998</v>
@@ -4019,25 +4215,25 @@
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1">
       <c r="A11" s="60" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C11" s="47">
         <v>44.071427999999997</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="60"/>
       <c r="B12" s="47" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C12" s="47">
         <v>4.8571419999999996</v>
@@ -4048,7 +4244,7 @@
     <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="A13" s="60"/>
       <c r="B13" s="47" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C13" s="47">
         <v>0</v>
@@ -4058,25 +4254,25 @@
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1">
       <c r="A14" s="60" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C14" s="47">
         <v>45.571427999999997</v>
       </c>
       <c r="D14" s="61" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E14" s="62" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1">
       <c r="A15" s="60"/>
       <c r="B15" s="47" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C15" s="47">
         <v>68</v>
@@ -4087,7 +4283,7 @@
     <row r="16" spans="1:5" ht="18.75" customHeight="1">
       <c r="A16" s="60"/>
       <c r="B16" s="47" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C16" s="47">
         <v>48.714284999999997</v>
@@ -4098,7 +4294,7 @@
     <row r="17" spans="1:5" ht="18.75" customHeight="1">
       <c r="A17" s="60"/>
       <c r="B17" s="47" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C17" s="47">
         <v>18.714285</v>
@@ -4109,7 +4305,7 @@
     <row r="18" spans="1:5" ht="18.75" customHeight="1">
       <c r="A18" s="60"/>
       <c r="B18" s="47" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C18" s="47">
         <v>14.571427999999999</v>
@@ -4120,7 +4316,7 @@
     <row r="19" spans="1:5" ht="18.75" customHeight="1">
       <c r="A19" s="60"/>
       <c r="B19" s="47" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C19" s="47">
         <v>62</v>
@@ -4130,25 +4326,25 @@
     </row>
     <row r="20" spans="1:5" ht="28.5" customHeight="1">
       <c r="A20" s="60" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C20" s="47">
         <v>37.428570999999998</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="28.5" customHeight="1">
       <c r="A21" s="60"/>
       <c r="B21" s="47" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C21" s="47">
         <v>44.928571000000005</v>
@@ -4159,7 +4355,7 @@
     <row r="22" spans="1:5" ht="28.5" customHeight="1">
       <c r="A22" s="60"/>
       <c r="B22" s="47" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C22" s="47">
         <v>68.142857000000006</v>
@@ -4169,25 +4365,25 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="60" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B23" s="47" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C23" s="47">
         <v>22.142856999999999</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="E23" s="62" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="60"/>
       <c r="B24" s="47" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C24" s="47">
         <v>28</v>
@@ -4198,7 +4394,7 @@
     <row r="25" spans="1:5">
       <c r="A25" s="60"/>
       <c r="B25" s="47" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C25" s="47">
         <v>27</v>
@@ -4209,7 +4405,7 @@
     <row r="26" spans="1:5">
       <c r="A26" s="60"/>
       <c r="B26" s="47" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C26" s="47">
         <v>14.642856500000001</v>
@@ -4220,7 +4416,7 @@
     <row r="27" spans="1:5">
       <c r="A27" s="60"/>
       <c r="B27" s="47" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C27" s="47">
         <v>39.571427999999997</v>
@@ -4231,7 +4427,7 @@
     <row r="28" spans="1:5">
       <c r="A28" s="60"/>
       <c r="B28" s="47" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C28" s="47">
         <v>6.571428</v>
@@ -4241,25 +4437,25 @@
     </row>
     <row r="29" spans="1:5" ht="38.25" customHeight="1">
       <c r="A29" s="60" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C29" s="47">
         <v>0.45488721804499999</v>
       </c>
       <c r="D29" s="61" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="38.25" customHeight="1">
       <c r="A30" s="60"/>
       <c r="B30" s="47" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C30" s="47">
         <v>3.8004750593E-2</v>
@@ -4270,7 +4466,7 @@
     <row r="31" spans="1:5" ht="38.25" customHeight="1">
       <c r="A31" s="60"/>
       <c r="B31" s="47" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C31" s="47">
         <v>5.6338028169E-2</v>
@@ -4280,10 +4476,10 @@
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1">
       <c r="A32" s="60" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -4292,7 +4488,7 @@
     <row r="33" spans="1:3">
       <c r="A33" s="60"/>
       <c r="B33" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C33">
         <v>52</v>
@@ -4301,7 +4497,7 @@
     <row r="34" spans="1:3">
       <c r="A34" s="60"/>
       <c r="B34" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C34">
         <v>10</v>
@@ -4309,10 +4505,10 @@
     </row>
     <row r="35" spans="1:3" ht="45" customHeight="1">
       <c r="A35" s="60" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B35" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -4321,7 +4517,7 @@
     <row r="36" spans="1:3">
       <c r="A36" s="60"/>
       <c r="B36" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -4330,7 +4526,7 @@
     <row r="37" spans="1:3">
       <c r="A37" s="60"/>
       <c r="B37" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -4338,10 +4534,10 @@
     </row>
     <row r="38" spans="1:3" ht="30" customHeight="1">
       <c r="A38" s="60" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B38" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -4350,7 +4546,7 @@
     <row r="39" spans="1:3">
       <c r="A39" s="60"/>
       <c r="B39" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -4358,10 +4554,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="60" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B40" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C40">
         <v>4</v>
@@ -4370,7 +4566,7 @@
     <row r="41" spans="1:3">
       <c r="A41" s="60"/>
       <c r="B41" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -4379,7 +4575,7 @@
     <row r="42" spans="1:3">
       <c r="A42" s="60"/>
       <c r="B42" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C42">
         <v>4</v>
@@ -4387,19 +4583,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="A29:A31"/>
     <mergeCell ref="E29:E31"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="E11:E13"/>
@@ -4409,12 +4598,19 @@
     <mergeCell ref="E14:E19"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E23:E28"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>